<commit_message>
commit after done with feedback 02/08
</commit_message>
<xml_diff>
--- a/src/assets/images/DEALTABLE_Long-list.xlsx
+++ b/src/assets/images/DEALTABLE_Long-list.xlsx
@@ -793,7 +793,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -832,12 +832,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -860,7 +854,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -876,16 +870,13 @@
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -894,19 +885,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -916,6 +895,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1202,14 +1193,14 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="14.19921875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.09765625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.19921875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.796875" customWidth="1"/>
@@ -1218,60 +1209,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="14" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="18" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="15"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="10"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
@@ -1281,31 +1272,31 @@
       <c r="C3" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="14">
         <v>19760401</v>
       </c>
       <c r="G3" s="4">
         <v>170.46312</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>214.52723</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>25.114560000000001</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="7" t="s">
+      <c r="J3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="17" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -1320,31 +1311,31 @@
       <c r="C4" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="14">
         <v>19831221</v>
       </c>
       <c r="G4" s="4">
         <v>331.20560999999998</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>299.00322</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>23.01595</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="7" t="s">
+      <c r="J4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="17" t="s">
         <v>18</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -1359,31 +1350,31 @@
       <c r="C5" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>54</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="14">
         <v>20100706</v>
       </c>
       <c r="G5" s="4">
         <v>102.22318</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>138.94845000000001</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>21.185220000000001</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="7" t="s">
+      <c r="J5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -1398,31 +1389,31 @@
       <c r="C6" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>66</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="14">
         <v>20010810</v>
       </c>
       <c r="G6" s="4">
         <v>380.93961999999999</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>475.31385</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>17.31634</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="7" t="s">
+      <c r="J6" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="17" t="s">
         <v>15</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -1437,31 +1428,31 @@
       <c r="C7" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>134</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="14">
         <v>19671020</v>
       </c>
       <c r="G7" s="4">
         <v>547.93742999999995</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>529.13661000000002</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>16.707419999999999</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="7" t="s">
+      <c r="J7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="17" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="2" t="s">
@@ -1475,31 +1466,31 @@
       <c r="C8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>51</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="14">
         <v>20050221</v>
       </c>
       <c r="G8" s="4">
         <v>281.64749999999998</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>268.83796999999998</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>28.496040000000001</v>
       </c>
-      <c r="J8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="7" t="s">
+      <c r="J8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="17" t="s">
         <v>28</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -1513,31 +1504,31 @@
       <c r="C9" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <v>73</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="14">
         <v>20020923</v>
       </c>
       <c r="G9" s="4">
         <v>435.79982999999999</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>372.58951000000002</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>28.234850000000002</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="7" t="s">
+      <c r="J9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="17" t="s">
         <v>33</v>
       </c>
       <c r="M9" s="2" t="s">
@@ -1551,31 +1542,31 @@
       <c r="C10" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>67</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="14">
         <v>19751220</v>
       </c>
       <c r="G10" s="4">
         <v>298.05286000000001</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>494.43416999999999</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>27.24766</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="7" t="s">
+      <c r="J10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="17" t="s">
         <v>36</v>
       </c>
       <c r="M10" s="2" t="s">
@@ -1589,31 +1580,31 @@
       <c r="C11" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <v>58</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="14">
         <v>19891010</v>
       </c>
       <c r="G11" s="4">
         <v>301.70443</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>385.87988000000001</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>25.702100000000002</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="7" t="s">
+      <c r="J11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="17" t="s">
         <v>39</v>
       </c>
       <c r="M11" s="2" t="s">
@@ -1627,31 +1618,31 @@
       <c r="C12" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>156</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="14">
         <v>19930826</v>
       </c>
       <c r="G12" s="4">
         <v>503.48651999999998</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>567.26987999999994</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="4">
         <v>22.494070000000001</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="7" t="s">
+      <c r="J12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="17" t="s">
         <v>42</v>
       </c>
       <c r="M12" s="2" t="s">
@@ -1665,31 +1656,31 @@
       <c r="C13" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="3">
         <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="14">
         <v>20031224</v>
       </c>
       <c r="G13" s="4">
         <v>159.00867</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <v>234.12949</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="4">
         <v>17.466249999999999</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="7" t="s">
+      <c r="J13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="17" t="s">
         <v>50</v>
       </c>
       <c r="M13" s="2" t="s">
@@ -1703,31 +1694,31 @@
       <c r="C14" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="3">
         <v>85</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="14">
         <v>19991022</v>
       </c>
       <c r="G14" s="4">
         <v>309.09616</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="4">
         <v>262.74712</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="4">
         <v>34.760260000000002</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" s="7" t="s">
+      <c r="J14" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="17" t="s">
         <v>55</v>
       </c>
       <c r="M14" s="2" t="s">
@@ -1741,31 +1732,31 @@
       <c r="C15" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="3">
         <v>78</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="14">
         <v>19670208</v>
       </c>
       <c r="G15" s="4">
         <v>326.77087</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <v>318.88733000000002</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="4">
         <v>13.523949999999999</v>
       </c>
-      <c r="J15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="7" t="s">
+      <c r="J15" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="17" t="s">
         <v>57</v>
       </c>
       <c r="M15" s="2" t="s">
@@ -1779,31 +1770,31 @@
       <c r="C16" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="3">
         <v>34</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="14">
         <v>19941004</v>
       </c>
       <c r="G16" s="4">
         <v>108.91912000000001</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="4">
         <v>129.42902000000001</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="4">
         <v>12.699310000000001</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" s="7" t="s">
+      <c r="J16" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="17" t="s">
         <v>15</v>
       </c>
       <c r="M16" s="2" t="s">
@@ -1817,31 +1808,31 @@
       <c r="C17" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="3">
         <v>82</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="14">
         <v>20000324</v>
       </c>
       <c r="G17" s="4">
         <v>295.16189000000003</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="4">
         <v>369.34244999999999</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="4">
         <v>10.09643</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="7" t="s">
+      <c r="J17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="17" t="s">
         <v>55</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -1855,31 +1846,31 @@
       <c r="C18" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="3">
         <v>218</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="14">
         <v>20011220</v>
       </c>
       <c r="G18" s="4">
         <v>349.65415000000002</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="4">
         <v>436.63596999999999</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="4">
         <v>39.906039999999997</v>
       </c>
-      <c r="J18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" s="7" t="s">
+      <c r="J18" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="17" t="s">
         <v>42</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -1893,31 +1884,31 @@
       <c r="C19" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="3">
         <v>37</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="14">
         <v>20010427</v>
       </c>
       <c r="G19" s="4">
         <v>348.15325999999999</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="4">
         <v>476.88085000000001</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="4">
         <v>35.861840000000001</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K19" s="7" t="s">
+      <c r="J19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="17" t="s">
         <v>66</v>
       </c>
       <c r="M19" s="2" t="s">
@@ -1931,31 +1922,31 @@
       <c r="C20" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="3">
         <v>116</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="14">
         <v>19870912</v>
       </c>
       <c r="G20" s="4">
         <v>447.78955000000002</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="4">
         <v>403.70238000000001</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="4">
         <v>35.260440000000003</v>
       </c>
-      <c r="J20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="7" t="s">
+      <c r="J20" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="17" t="s">
         <v>36</v>
       </c>
       <c r="M20" s="2" t="s">
@@ -1969,31 +1960,31 @@
       <c r="C21" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="3">
         <v>45</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="14">
         <v>19880802</v>
       </c>
       <c r="G21" s="4">
         <v>200.21728999999999</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="4">
         <v>148.62826999999999</v>
       </c>
-      <c r="I21" s="5">
-        <v>12</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K21" s="7" t="s">
+      <c r="I21" s="4">
+        <v>12</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="L21" s="17" t="s">
         <v>28</v>
       </c>
       <c r="M21" s="2" t="s">
@@ -2007,31 +1998,31 @@
       <c r="C22" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="3">
         <v>37</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="14">
         <v>19830809</v>
       </c>
       <c r="G22" s="4">
         <v>118.80916000000001</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="4">
         <v>110.74737</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="4">
         <v>15</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K22" s="7" t="s">
+      <c r="J22" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="L22" s="17" t="s">
         <v>39</v>
       </c>
       <c r="M22" s="2" t="s">
@@ -2045,31 +2036,31 @@
       <c r="C23" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="3">
         <v>69</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="14">
         <v>20221219</v>
       </c>
       <c r="G23" s="4">
         <v>185.74735999999999</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="4">
         <v>327.55606</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="4">
         <v>32.256709999999998</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K23" s="7" t="s">
+      <c r="J23" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="17" t="s">
         <v>70</v>
       </c>
       <c r="M23" s="2" t="s">
@@ -2083,31 +2074,31 @@
       <c r="C24" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="3">
         <v>33</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="14">
         <v>20220429</v>
       </c>
       <c r="G24" s="4">
         <v>120.04394000000001</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="4">
         <v>188.97554</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="4">
         <v>10</v>
       </c>
-      <c r="J24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K24" s="7" t="s">
+      <c r="J24" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="L24" s="17" t="s">
         <v>70</v>
       </c>
       <c r="M24" s="2" t="s">
@@ -2121,31 +2112,31 @@
       <c r="C25" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="3">
         <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="14">
         <v>20170915</v>
       </c>
       <c r="G25" s="4">
         <v>118.32659</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="4">
         <v>131.18489</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="4">
         <v>10.641579999999999</v>
       </c>
-      <c r="J25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K25" s="7" t="s">
+      <c r="J25" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="L25" s="17" t="s">
         <v>75</v>
       </c>
       <c r="M25" s="2" t="s">
@@ -2159,31 +2150,31 @@
       <c r="C26" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="3">
         <v>49</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="14">
         <v>20111122</v>
       </c>
       <c r="G26" s="4">
         <v>244.30193</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="4">
         <v>296.98128000000003</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="4">
         <v>29.555900000000001</v>
       </c>
-      <c r="J26" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K26" s="7" t="s">
+      <c r="J26" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="L26" s="17" t="s">
         <v>42</v>
       </c>
       <c r="M26" s="2" t="s">
@@ -2197,31 +2188,31 @@
       <c r="C27" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="3">
         <v>36</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="14">
         <v>20150911</v>
       </c>
       <c r="G27" s="4">
         <v>211.51772</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27" s="4">
         <v>178.93801999999999</v>
       </c>
-      <c r="I27" s="5">
+      <c r="I27" s="4">
         <v>10.95438</v>
       </c>
-      <c r="J27" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K27" s="7" t="s">
+      <c r="J27" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="L27" s="8" t="s">
+      <c r="L27" s="17" t="s">
         <v>62</v>
       </c>
       <c r="M27" s="2" t="s">
@@ -2235,31 +2226,31 @@
       <c r="C28" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="3">
         <v>36</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="14">
         <v>20140416</v>
       </c>
       <c r="G28" s="4">
         <v>162.17429999999999</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="4">
         <v>194.7039</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I28" s="4">
         <v>15.573740000000001</v>
       </c>
-      <c r="J28" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K28" s="7" t="s">
+      <c r="J28" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="L28" s="17" t="s">
         <v>42</v>
       </c>
       <c r="M28" s="2" t="s">
@@ -2273,31 +2264,31 @@
       <c r="C29" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="3">
         <v>23</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="14">
         <v>20120326</v>
       </c>
       <c r="G29" s="4">
         <v>160.38918000000001</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="4">
         <v>219.83282</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I29" s="4">
         <v>20.031610000000001</v>
       </c>
-      <c r="J29" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K29" s="7" t="s">
+      <c r="J29" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="L29" s="17" t="s">
         <v>42</v>
       </c>
       <c r="M29" s="2" t="s">
@@ -2311,31 +2302,31 @@
       <c r="C30" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="3">
         <v>34</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="14">
         <v>20131224</v>
       </c>
       <c r="G30" s="4">
         <v>175.85182</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H30" s="4">
         <v>171.99646000000001</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I30" s="4">
         <v>18.946249999999999</v>
       </c>
-      <c r="J30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K30" s="7" t="s">
+      <c r="J30" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="L30" s="17" t="s">
         <v>47</v>
       </c>
       <c r="M30" s="2" t="s">
@@ -2349,31 +2340,31 @@
       <c r="C31" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="3">
         <v>9</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="14">
         <v>20191231</v>
       </c>
       <c r="G31" s="4">
         <v>87.647180000000006</v>
       </c>
-      <c r="H31" s="5">
+      <c r="H31" s="4">
         <v>156.76420999999999</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I31" s="4">
         <v>28.88674</v>
       </c>
-      <c r="J31" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" s="7" t="s">
+      <c r="J31" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="L31" s="17" t="s">
         <v>28</v>
       </c>
       <c r="M31" s="2" t="s">
@@ -2387,31 +2378,31 @@
       <c r="C32" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="3">
         <v>23</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="14">
         <v>20110303</v>
       </c>
       <c r="G32" s="4">
         <v>73.062870000000004</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32" s="4">
         <v>126.98090000000001</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I32" s="4">
         <v>13</v>
       </c>
-      <c r="J32" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K32" s="7" t="s">
+      <c r="J32" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="L32" s="17" t="s">
         <v>39</v>
       </c>
       <c r="M32" s="2" t="s">
@@ -2425,31 +2416,31 @@
       <c r="C33" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="3">
         <v>20</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33" s="14">
         <v>20110822</v>
       </c>
       <c r="G33" s="4">
         <v>116.61682999999999</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H33" s="4">
         <v>131.49405999999999</v>
       </c>
       <c r="I33" s="4">
         <v>8.2891999999999992</v>
       </c>
-      <c r="J33" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K33" s="7" t="s">
+      <c r="J33" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="L33" s="17" t="s">
         <v>39</v>
       </c>
       <c r="M33" s="2" t="s">
@@ -2463,31 +2454,31 @@
       <c r="C34" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="3">
         <v>39</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="14">
         <v>20130925</v>
       </c>
       <c r="G34" s="4">
         <v>119.98069</v>
       </c>
-      <c r="H34" s="5">
+      <c r="H34" s="4">
         <v>258.76553000000001</v>
       </c>
       <c r="I34" s="4">
         <v>8</v>
       </c>
-      <c r="J34" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K34" s="7" t="s">
+      <c r="J34" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K34" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="L34" s="3" t="s">
+      <c r="L34" s="17" t="s">
         <v>42</v>
       </c>
       <c r="M34" s="2" t="s">

</xml_diff>